<commit_message>
added README; updated 501283 and 501419
</commit_message>
<xml_diff>
--- a/nmadb/501283.xlsx
+++ b/nmadb/501283.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagiaire_2018\Desktop\nmadata\nmadb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21255" windowHeight="9990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -264,8 +269,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +297,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,16 +319,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -364,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,9 +416,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,6 +451,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -605,16 +627,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +665,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1984</v>
       </c>
@@ -674,7 +696,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>1</v>
       </c>
@@ -696,7 +718,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1999</v>
       </c>
@@ -724,7 +746,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -746,7 +768,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1992</v>
       </c>
@@ -774,7 +796,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -796,7 +818,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1990</v>
       </c>
@@ -824,7 +846,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>4</v>
       </c>
@@ -846,7 +868,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1984</v>
       </c>
@@ -874,7 +896,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>5</v>
       </c>
@@ -896,7 +918,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>5</v>
       </c>
@@ -918,7 +940,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1986</v>
       </c>
@@ -946,7 +968,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>6</v>
       </c>
@@ -968,7 +990,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1992</v>
       </c>
@@ -996,7 +1018,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>7</v>
       </c>
@@ -1018,7 +1040,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1976</v>
       </c>
@@ -1046,7 +1068,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>8</v>
       </c>
@@ -1068,7 +1090,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1994</v>
       </c>
@@ -1088,7 +1110,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>9</v>
       </c>
@@ -1102,7 +1124,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2000</v>
       </c>
@@ -1122,7 +1144,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>10</v>
       </c>
@@ -1136,7 +1158,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2007</v>
       </c>
@@ -1156,7 +1178,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>11</v>
       </c>
@@ -1170,7 +1192,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
@@ -1190,7 +1212,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>12</v>
       </c>
@@ -1204,7 +1226,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1991</v>
       </c>
@@ -1224,7 +1246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>13</v>
       </c>
@@ -1238,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1989</v>
       </c>
@@ -1258,7 +1280,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>14</v>
       </c>
@@ -1272,7 +1294,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1991</v>
       </c>
@@ -1292,7 +1314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>15</v>
       </c>
@@ -1306,7 +1328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -1326,7 +1348,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>16</v>
       </c>
@@ -1340,7 +1362,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1984</v>
       </c>
@@ -1360,7 +1382,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>17</v>
       </c>
@@ -1374,7 +1396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1988</v>
       </c>
@@ -1394,7 +1416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>18</v>
       </c>
@@ -1408,7 +1430,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1985</v>
       </c>
@@ -1428,7 +1450,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>19</v>
       </c>
@@ -1442,7 +1464,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>19</v>
       </c>
@@ -1456,7 +1478,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1999</v>
       </c>
@@ -1476,7 +1498,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>20</v>
       </c>
@@ -1490,7 +1512,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2006</v>
       </c>
@@ -1510,7 +1532,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>21</v>
       </c>
@@ -1524,7 +1546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2007</v>
       </c>
@@ -1544,7 +1566,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>22</v>
       </c>
@@ -1558,7 +1580,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1999</v>
       </c>
@@ -1578,7 +1600,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>23</v>
       </c>
@@ -1592,7 +1614,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1993</v>
       </c>
@@ -1612,7 +1634,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>24</v>
       </c>
@@ -1626,7 +1648,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1990</v>
       </c>
@@ -1646,7 +1668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>25</v>
       </c>
@@ -1660,7 +1682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1992</v>
       </c>
@@ -1680,7 +1702,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>26</v>
       </c>
@@ -1694,7 +1716,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2001</v>
       </c>
@@ -1714,7 +1736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>27</v>
       </c>
@@ -1728,7 +1750,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2004</v>
       </c>
@@ -1748,7 +1770,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>28</v>
       </c>
@@ -1762,7 +1784,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2007</v>
       </c>
@@ -1782,7 +1804,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>29</v>
       </c>
@@ -1796,7 +1818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2007</v>
       </c>
@@ -1816,7 +1838,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>30</v>
       </c>
@@ -1830,7 +1852,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1998</v>
       </c>
@@ -1850,7 +1872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>31</v>
       </c>
@@ -1864,7 +1886,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2008</v>
       </c>
@@ -1884,7 +1906,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>32</v>
       </c>
@@ -1898,7 +1920,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2003</v>
       </c>
@@ -1918,7 +1940,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>33</v>
       </c>
@@ -1932,7 +1954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2000</v>
       </c>
@@ -1952,7 +1974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>34</v>
       </c>
@@ -1966,7 +1988,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1997</v>
       </c>
@@ -1986,7 +2008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>35</v>
       </c>
@@ -2000,7 +2022,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1998</v>
       </c>
@@ -2020,7 +2042,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C75">
         <v>36</v>
       </c>
@@ -2034,7 +2056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1993</v>
       </c>
@@ -2054,7 +2076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C77">
         <v>37</v>
       </c>
@@ -2068,7 +2090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2009</v>
       </c>
@@ -2088,7 +2110,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C79">
         <v>38</v>
       </c>
@@ -2102,7 +2124,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2006</v>
       </c>
@@ -2122,7 +2144,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C81">
         <v>39</v>
       </c>
@@ -2136,7 +2158,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2000</v>
       </c>
@@ -2156,7 +2178,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C83">
         <v>40</v>
       </c>
@@ -2170,7 +2192,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2007</v>
       </c>
@@ -2190,7 +2212,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C85">
         <v>41</v>
       </c>
@@ -2204,7 +2226,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2002</v>
       </c>
@@ -2224,7 +2246,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C87">
         <v>42</v>
       </c>
@@ -2238,7 +2260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2008</v>
       </c>
@@ -2258,7 +2280,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C89">
         <v>43</v>
       </c>
@@ -2272,7 +2294,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2007</v>
       </c>
@@ -2292,7 +2314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>44</v>
       </c>
@@ -2306,7 +2328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2005</v>
       </c>
@@ -2326,7 +2348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>45</v>
       </c>
@@ -2340,7 +2362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2006</v>
       </c>
@@ -2360,7 +2382,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>46</v>
       </c>
@@ -2374,7 +2396,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2003</v>
       </c>
@@ -2394,7 +2416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>47</v>
       </c>
@@ -2408,7 +2430,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2001</v>
       </c>
@@ -2428,7 +2450,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>48</v>
       </c>
@@ -2442,7 +2464,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2008</v>
       </c>
@@ -2462,7 +2484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>49</v>
       </c>
@@ -2476,7 +2498,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2001</v>
       </c>
@@ -2496,7 +2518,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>50</v>
       </c>
@@ -2510,7 +2532,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1979</v>
       </c>
@@ -2530,7 +2552,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>51</v>
       </c>
@@ -2544,7 +2566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2009</v>
       </c>
@@ -2564,7 +2586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>52</v>
       </c>
@@ -2578,7 +2600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2010</v>
       </c>
@@ -2598,7 +2620,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>53</v>
       </c>
@@ -2612,7 +2634,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2011</v>
       </c>
@@ -2625,28 +2647,28 @@
       <c r="D110">
         <v>2</v>
       </c>
-      <c r="E110">
-        <v>16.5</v>
+      <c r="E110" s="3">
+        <v>1</v>
       </c>
       <c r="F110">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C111">
         <v>54</v>
       </c>
       <c r="D111">
         <v>6</v>
       </c>
-      <c r="E111">
-        <v>30.5</v>
+      <c r="E111" s="3">
+        <v>4</v>
       </c>
       <c r="F111">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2009</v>
       </c>
@@ -2666,7 +2688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="3:6">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C113">
         <v>55</v>
       </c>
@@ -2686,24 +2708,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>